<commit_message>
fix: deal with a bug in the worksheet provided by the licitanet portal
</commit_message>
<xml_diff>
--- a/PropProAssistant/Test/WorksheetModels/LicitaNet/LN_01.xlsx
+++ b/PropProAssistant/Test/WorksheetModels/LicitaNet/LN_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DotNETProjects\proppro-assistant\PropProAssistant\Models\LicitaNet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54cd02815d7cac6c/Documentos/Projetos/proppro-assistant/PropProAssistant/Test/WorksheetModels/LicitaNet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF6C64F-A418-4138-A0EB-7513FFFBFEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6FF6C64F-A418-4138-A0EB-7513FFFBFEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CED886E-ADC9-4A49-B647-556620A203D0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>LOTE</t>
   </si>
@@ -61,27 +61,15 @@
     <t>AMINOFILINA - PRINCÍPIO ATIVO: AMINOFILINA; CONCENTRAÇÃO/DOSAGEM: 24MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 10ML</t>
   </si>
   <si>
-    <t>Farmace</t>
-  </si>
-  <si>
     <t>AMIODARONA - PRINCIPIO ATIVO: AMIODARONA; CONCENTRACAO/DOSAGEM: 50 MG/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 3 ML.</t>
   </si>
   <si>
-    <t>Hipolabor</t>
-  </si>
-  <si>
     <t>AMOXICILINA - PRINCIPIO ATIVO: AMOXICILINA; CONCENTRACAO/DOSAGEM: 250 MG/5 ML; FORMA FARMACEUTICA: PO PARA SUSPENSAO ORAL; APRESENTACAO: FRASCO 60ML; COMPONENTE: COPO MEDIDOR;</t>
   </si>
   <si>
-    <t>Hypofarma</t>
-  </si>
-  <si>
     <t>AMOXICILINA + ASSOCIACOES - PRINCIPIO ATIVO: AMOXICILINA + CLAVULANATO DE POTASSIO; CONCENTRACAO/DOSAGEM: 50 MG/ML + 12,5 MG/ML; FORMA FARMACEUTICA: PO PARA SUSPENSAO ORAL; APRESENTACAO: FRASCO 75 ML; COMPONENTE: DOSADOR;</t>
   </si>
   <si>
-    <t>Isofarma</t>
-  </si>
-  <si>
     <t>AMOXICILINA + ASSOCIACOES - PRINCIPIO ATIVO: AMOXICILINA + CLAVULANATO DE POTASSIO; CONCENTRACAO/DOSAGEM: 500 MG + 125 MG; FORMA FARMACEUTICA: COMPRIMIDO REVESTIDO.</t>
   </si>
   <si>
@@ -91,9 +79,6 @@
     <t>ATROPINA - PRINCIPIO ATIVO: ATROPINA, SULFATO; CONCENTRACAO/DOSAGEM: 0,25 MG/ML; FORMA FARMACEUTICA: SOLUCAO INJETAVEL; APRESENTACAO: AMPOLA 1 ML.</t>
   </si>
   <si>
-    <t>EMS</t>
-  </si>
-  <si>
     <t>AZITROMICINA - PRINCIPIO ATIVO: AZITROMICINA DI-HIDRATADA; CONCENTRACAO/DOSAGEM: 200 MG/5 ML; FORMA FARMACEUTICA: PO PARA SUSPENSAO ORAL; APRESENTACAO: FRASCO 15 ML; COMPONENTE: FRASCO DILUENTE + SERINGA DOSADORA;</t>
   </si>
   <si>
@@ -124,9 +109,6 @@
     <t>CLONAZEPAM - PRINCIPIO ATIVO: CLONAZEPAM; CONCENTRACAO/DOSAGEM: 2,5 MG/ML; FORMA FARMACEUTICA: SOLUCAO ORAL; APRESENTACAO: FRASCO 20 ML.</t>
   </si>
   <si>
-    <t>Teuto</t>
-  </si>
-  <si>
     <t>CLOPIDOGREL - PRINCÍPIO ATIVO:CLOPIDOGREL; CONCENTRAÇÃO DOSAGEM: 75MG; FORMA FAMACÊUTICA: COMPRIMIDOS RESVESTIDOS; APRESENTAÇÃO: CAIXA DE 28 A 56 COMPRIMIDOS</t>
   </si>
   <si>
@@ -169,9 +151,6 @@
     <t>DIFENIDRAMINA - PRINCÍPIO ATIVO: DIFENIDRAMINA; CONCENTRAÇÃO/DOSAGEM: 50MG/ML; FORMA FARMACÊUTICA: SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 1ML.</t>
   </si>
   <si>
-    <t>Blau</t>
-  </si>
-  <si>
     <t xml:space="preserve">DIGOXINA - PRINCIPIO ATIVO: DIGOXINA; CONCENTRACAO/DOSAGEM: 0,25 MG; FORMA FARMACEUTICA: COMPRIMIDO. </t>
   </si>
   <si>
@@ -256,15 +235,9 @@
     <t>HIPROMELOSE - PRINCIPIO ATIVO: HIPROMELOSE; CONCENTRACAO/DOSAGEM: 5 MG/ML; FORMA FARMACEUTICA: SOLUCAO OFTALMICA; APRESENTACAO: FRASCO 10 ML.</t>
   </si>
   <si>
-    <t>Sanval</t>
-  </si>
-  <si>
     <t xml:space="preserve">HYPLEX - PRINCÍPIO ATIVO: COMPLEXO B; FORMA FARMACÊUTICA:  SOLUÇÃO INJETÁVEL; APRESENTAÇÃO: AMPOLAS 2ML.</t>
   </si>
   <si>
-    <t>Cristália</t>
-  </si>
-  <si>
     <t>IBUPROFENO - PRINCIPIO ATIVO: IBUPROFENO; CONCENTRACAO/DOSAGEM: 100 MG/ML; FORMA FARMACEUTICA: SUSPENSAO ORAL (GOTAS); APRESENTACAO: FRASCO 30 ML.</t>
   </si>
   <si>
@@ -292,9 +265,6 @@
     <t>METILPREDNISOLONA - PRINCÍPIO ATIVO: SUCCINATO SÓDICO DE METILPREDNISOLONA; CONCENTRAÇÃO/DOSAGEM: 500MG; FORMA FARMACÊUTICA: PÓ PARA SOLUÇÃO IM OU IV; APRESENTAÇÃO: CAIXA COM 25 FRASCOS; COMPONENTE: DILUENTE 8ML.</t>
   </si>
   <si>
-    <t>Takeda</t>
-  </si>
-  <si>
     <t>METOCLOPRAMIDA - PRINCIPIO ATIVO: METOCLOPRAMIDA, CLORIDRATO; CONCENTRACAO/DOSAGEM: 4 MG/ML; FORMA FARMACEUTICA: SOLUCAO ORAL; APRESENTACAO: FRASCO 10 ML.</t>
   </si>
   <si>
@@ -320,9 +290,6 @@
   </si>
   <si>
     <t>NIMESULIDA - PRINCÍPIO ATIVO: NIMESULIDA; CONCENTRAÇÃO/DOSAGEM: 100MG; FORMA FARMACÊUTICA: COMPRIMIDOS; APRESENTAÇÃO: BLISTER COM 10 OU 12 COMPRIMIDOS.</t>
-  </si>
-  <si>
-    <t>Mylan</t>
   </si>
   <si>
     <t>NISTATINA - PRINCÍPIO ATIVO: NISTATINA; CONCENTRAÇÃO/DOSAGEM: 25.000UI/G; FORMA FARMACÊUTICA: CREME VAGINAL; APRESENTAÇÃO: BISNAGA 60G; COMPONENTE: COM APLICADORES.</t>
@@ -443,12 +410,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,6 +755,8 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" ht="45">
       <c r="A2" s="0">
@@ -807,8 +777,8 @@
       <c r="F2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2">
-        <v>0</v>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" ht="45">
@@ -830,8 +800,8 @@
       <c r="F3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="2">
-        <v>0</v>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" ht="45">
@@ -853,8 +823,8 @@
       <c r="F4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="2">
-        <v>0</v>
+      <c r="G4" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" ht="45">
@@ -871,13 +841,13 @@
         <v>100</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="2">
-        <v>4.42</v>
+        <v>8</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" ht="45">
@@ -888,19 +858,19 @@
         <v>3143320</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2">
         <v>100</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="2">
-        <v>7.15</v>
+        <v>8</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" ht="60">
@@ -911,19 +881,19 @@
         <v>3143321</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2">
         <v>600</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2.99</v>
+        <v>8</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" ht="60">
@@ -934,19 +904,19 @@
         <v>3143322</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2">
         <v>100</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.65</v>
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" ht="45">
@@ -957,7 +927,7 @@
         <v>3143323</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2">
         <v>1500</v>
@@ -968,8 +938,8 @@
       <c r="F9" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="2">
-        <v>0</v>
+      <c r="G9" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" ht="30">
@@ -980,19 +950,19 @@
         <v>3143324</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2">
         <v>1000</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="2">
-        <v>12.87</v>
+        <v>8</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" ht="45">
@@ -1003,19 +973,19 @@
         <v>3143325</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2">
         <v>100</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="2">
-        <v>76.7</v>
+        <v>8</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" ht="60">
@@ -1026,7 +996,7 @@
         <v>3143326</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2">
         <v>600</v>
@@ -1037,8 +1007,8 @@
       <c r="F12" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="2">
-        <v>0</v>
+      <c r="G12" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" ht="45">
@@ -1049,7 +1019,7 @@
         <v>3143327</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D13" s="2">
         <v>200</v>
@@ -1060,8 +1030,8 @@
       <c r="F13" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="2">
-        <v>0</v>
+      <c r="G13" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" ht="45">
@@ -1072,7 +1042,7 @@
         <v>3143328</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D14" s="2">
         <v>100</v>
@@ -1083,8 +1053,8 @@
       <c r="F14" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="2">
-        <v>0</v>
+      <c r="G14" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" ht="30">
@@ -1095,7 +1065,7 @@
         <v>3143329</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2">
         <v>5000</v>
@@ -1106,8 +1076,8 @@
       <c r="F15" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="2">
-        <v>0</v>
+      <c r="G15" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" ht="30">
@@ -1118,7 +1088,7 @@
         <v>3143330</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2">
         <v>4000</v>
@@ -1129,8 +1099,8 @@
       <c r="F16" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="2">
-        <v>0</v>
+      <c r="G16" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" ht="45">
@@ -1141,7 +1111,7 @@
         <v>3143331</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D17" s="2">
         <v>400</v>
@@ -1152,8 +1122,8 @@
       <c r="F17" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="2">
-        <v>0</v>
+      <c r="G17" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18" ht="45">
@@ -1164,7 +1134,7 @@
         <v>3143332</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2">
         <v>6000</v>
@@ -1175,8 +1145,8 @@
       <c r="F18" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="2">
-        <v>0</v>
+      <c r="G18" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="19" ht="45">
@@ -1187,7 +1157,7 @@
         <v>3143333</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D19" s="2">
         <v>1000</v>
@@ -1198,8 +1168,8 @@
       <c r="F19" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="2">
-        <v>0</v>
+      <c r="G19" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="20" ht="45">
@@ -1210,7 +1180,7 @@
         <v>3143334</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D20" s="2">
         <v>12000</v>
@@ -1221,8 +1191,8 @@
       <c r="F20" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="2">
-        <v>0</v>
+      <c r="G20" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" ht="45">
@@ -1233,19 +1203,19 @@
         <v>3143335</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2">
         <v>600</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="2">
-        <v>12.35</v>
+        <v>8</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="22" ht="45">
@@ -1256,7 +1226,7 @@
         <v>3143336</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2">
         <v>2000</v>
@@ -1267,8 +1237,8 @@
       <c r="F22" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="2">
-        <v>0</v>
+      <c r="G22" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23" ht="45">
@@ -1279,7 +1249,7 @@
         <v>3143337</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D23" s="2">
         <v>100</v>
@@ -1290,8 +1260,8 @@
       <c r="F23" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="2">
-        <v>0</v>
+      <c r="G23" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="24" ht="45">
@@ -1302,7 +1272,7 @@
         <v>3143338</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D24" s="2">
         <v>600</v>
@@ -1313,8 +1283,8 @@
       <c r="F24" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="2">
-        <v>0</v>
+      <c r="G24" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="25" ht="30">
@@ -1325,7 +1295,7 @@
         <v>3143339</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D25" s="2">
         <v>1000</v>
@@ -1336,8 +1306,8 @@
       <c r="F25" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="2">
-        <v>0</v>
+      <c r="G25" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="26" ht="45">
@@ -1348,7 +1318,7 @@
         <v>3143340</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D26" s="2">
         <v>100</v>
@@ -1359,8 +1329,8 @@
       <c r="F26" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="2">
-        <v>0</v>
+      <c r="G26" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="27" ht="45">
@@ -1371,19 +1341,19 @@
         <v>3143341</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D27" s="2">
         <v>20</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="2">
-        <v>3.38</v>
+        <v>8</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" ht="45">
@@ -1394,7 +1364,7 @@
         <v>3143342</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D28" s="2">
         <v>100</v>
@@ -1405,8 +1375,8 @@
       <c r="F28" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="2">
-        <v>0</v>
+      <c r="G28" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="29" ht="45">
@@ -1417,7 +1387,7 @@
         <v>3143343</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D29" s="2">
         <v>600</v>
@@ -1428,8 +1398,8 @@
       <c r="F29" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="2">
-        <v>0</v>
+      <c r="G29" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="30" ht="45">
@@ -1440,7 +1410,7 @@
         <v>3143344</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D30" s="2">
         <v>800</v>
@@ -1451,8 +1421,8 @@
       <c r="F30" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="2">
-        <v>0</v>
+      <c r="G30" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="31" ht="45">
@@ -1463,7 +1433,7 @@
         <v>3143345</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D31" s="2">
         <v>1000</v>
@@ -1474,8 +1444,8 @@
       <c r="F31" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="2">
-        <v>0</v>
+      <c r="G31" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="32" ht="45">
@@ -1486,7 +1456,7 @@
         <v>3143346</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D32" s="2">
         <v>200</v>
@@ -1497,8 +1467,8 @@
       <c r="F32" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="2">
-        <v>0</v>
+      <c r="G32" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="33" ht="45">
@@ -1509,7 +1479,7 @@
         <v>3143347</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D33" s="2">
         <v>1000</v>
@@ -1520,8 +1490,8 @@
       <c r="F33" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="2">
-        <v>0</v>
+      <c r="G33" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="34" ht="45">
@@ -1532,7 +1502,7 @@
         <v>3143348</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D34" s="2">
         <v>10000</v>
@@ -1543,8 +1513,8 @@
       <c r="F34" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="2">
-        <v>0</v>
+      <c r="G34" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="35" ht="45">
@@ -1555,19 +1525,19 @@
         <v>3143349</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D35" s="2">
         <v>100</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G35" s="2">
-        <v>8.97</v>
+        <v>8</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="36" ht="30">
@@ -1578,19 +1548,19 @@
         <v>3143350</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D36" s="2">
         <v>1000</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G36" s="2">
-        <v>17.55</v>
+        <v>8</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="37" ht="30">
@@ -1601,19 +1571,19 @@
         <v>3143351</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D37" s="2">
         <v>1000</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G37" s="2">
-        <v>6.37</v>
+        <v>8</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="38" ht="60">
@@ -1624,7 +1594,7 @@
         <v>3143352</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D38" s="2">
         <v>200</v>
@@ -1635,8 +1605,8 @@
       <c r="F38" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G38" s="2">
-        <v>0</v>
+      <c r="G38" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="39" ht="60">
@@ -1647,7 +1617,7 @@
         <v>3143353</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D39" s="2">
         <v>400</v>
@@ -1658,8 +1628,8 @@
       <c r="F39" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="2">
-        <v>0</v>
+      <c r="G39" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="40" ht="45">
@@ -1670,7 +1640,7 @@
         <v>3143354</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D40" s="2">
         <v>30000</v>
@@ -1681,8 +1651,8 @@
       <c r="F40" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="2">
-        <v>0</v>
+      <c r="G40" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="41" ht="45">
@@ -1693,19 +1663,19 @@
         <v>3143355</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D41" s="2">
         <v>1000</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G41" s="2">
-        <v>3.25</v>
+        <v>8</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="42" ht="45">
@@ -1716,7 +1686,7 @@
         <v>3143356</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D42" s="2">
         <v>1000</v>
@@ -1727,8 +1697,8 @@
       <c r="F42" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="2">
-        <v>0</v>
+      <c r="G42" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="43" ht="45">
@@ -1739,19 +1709,19 @@
         <v>3143357</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D43" s="2">
         <v>100</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" s="2">
-        <v>44.2</v>
+        <v>8</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="44" ht="45">
@@ -1762,7 +1732,7 @@
         <v>3143358</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D44" s="2">
         <v>100</v>
@@ -1773,8 +1743,8 @@
       <c r="F44" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G44" s="2">
-        <v>0</v>
+      <c r="G44" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="45" ht="60">
@@ -1785,7 +1755,7 @@
         <v>3143359</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D45" s="2">
         <v>200</v>
@@ -1796,8 +1766,8 @@
       <c r="F45" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G45" s="2">
-        <v>0</v>
+      <c r="G45" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="46" ht="45">
@@ -1808,7 +1778,7 @@
         <v>3143360</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D46" s="2">
         <v>200</v>
@@ -1819,8 +1789,8 @@
       <c r="F46" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G46" s="2">
-        <v>0</v>
+      <c r="G46" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="47" ht="45">
@@ -1831,7 +1801,7 @@
         <v>3143361</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D47" s="2">
         <v>400</v>
@@ -1842,8 +1812,8 @@
       <c r="F47" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G47" s="2">
-        <v>0</v>
+      <c r="G47" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="48" ht="30">
@@ -1854,7 +1824,7 @@
         <v>3143362</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D48" s="2">
         <v>8000</v>
@@ -1865,8 +1835,8 @@
       <c r="F48" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G48" s="2">
-        <v>0</v>
+      <c r="G48" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="49" ht="45">
@@ -1877,7 +1847,7 @@
         <v>3143363</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D49" s="2">
         <v>100</v>
@@ -1888,8 +1858,8 @@
       <c r="F49" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G49" s="2">
-        <v>0</v>
+      <c r="G49" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="50" ht="45">
@@ -1900,7 +1870,7 @@
         <v>3143364</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D50" s="2">
         <v>12000</v>
@@ -1911,8 +1881,8 @@
       <c r="F50" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G50" s="2">
-        <v>0</v>
+      <c r="G50" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="51" ht="45">
@@ -1923,7 +1893,7 @@
         <v>3143365</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D51" s="2">
         <v>100</v>
@@ -1934,8 +1904,8 @@
       <c r="F51" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G51" s="2">
-        <v>0</v>
+      <c r="G51" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="52" ht="45">
@@ -1946,7 +1916,7 @@
         <v>3143366</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D52" s="2">
         <v>200</v>
@@ -1957,8 +1927,8 @@
       <c r="F52" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G52" s="2">
-        <v>0</v>
+      <c r="G52" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="53" ht="75">
@@ -1969,7 +1939,7 @@
         <v>3143367</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D53" s="2">
         <v>100</v>
@@ -1980,8 +1950,8 @@
       <c r="F53" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G53" s="2">
-        <v>0</v>
+      <c r="G53" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="54" ht="60">
@@ -1992,7 +1962,7 @@
         <v>3143368</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D54" s="2">
         <v>1000</v>
@@ -2003,8 +1973,8 @@
       <c r="F54" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G54" s="2">
-        <v>0</v>
+      <c r="G54" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="55" ht="45">
@@ -2015,7 +1985,7 @@
         <v>3143369</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D55" s="2">
         <v>200</v>
@@ -2026,8 +1996,8 @@
       <c r="F55" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G55" s="2">
-        <v>0</v>
+      <c r="G55" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="56" ht="45">
@@ -2038,7 +2008,7 @@
         <v>3143370</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D56" s="2">
         <v>100</v>
@@ -2049,8 +2019,8 @@
       <c r="F56" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G56" s="2">
-        <v>0</v>
+      <c r="G56" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="57" ht="30">
@@ -2061,7 +2031,7 @@
         <v>3143371</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D57" s="2">
         <v>5000</v>
@@ -2072,8 +2042,8 @@
       <c r="F57" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G57" s="2">
-        <v>0</v>
+      <c r="G57" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="58" ht="45">
@@ -2084,7 +2054,7 @@
         <v>3143372</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D58" s="2">
         <v>600</v>
@@ -2095,8 +2065,8 @@
       <c r="F58" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G58" s="2">
-        <v>0</v>
+      <c r="G58" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="59" ht="45">
@@ -2107,7 +2077,7 @@
         <v>3143373</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D59" s="2">
         <v>600</v>
@@ -2118,8 +2088,8 @@
       <c r="F59" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="2">
-        <v>0</v>
+      <c r="G59" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="60" ht="45">
@@ -2130,7 +2100,7 @@
         <v>3143374</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D60" s="2">
         <v>100</v>
@@ -2141,8 +2111,8 @@
       <c r="F60" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G60" s="2">
-        <v>0</v>
+      <c r="G60" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="61" ht="60">
@@ -2153,7 +2123,7 @@
         <v>3143375</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D61" s="2">
         <v>100</v>
@@ -2164,8 +2134,8 @@
       <c r="F61" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G61" s="2">
-        <v>0</v>
+      <c r="G61" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="62" ht="45">
@@ -2176,7 +2146,7 @@
         <v>3143376</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D62" s="2">
         <v>200</v>
@@ -2187,8 +2157,8 @@
       <c r="F62" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G62" s="2">
-        <v>0</v>
+      <c r="G62" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="63" ht="45">
@@ -2199,19 +2169,19 @@
         <v>3143377</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D63" s="2">
         <v>20</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="G63" s="2">
-        <v>3.9</v>
+        <v>8</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="64" ht="30">
@@ -2222,19 +2192,19 @@
         <v>3143378</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D64" s="2">
         <v>1000</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="G64" s="2">
-        <v>10.4</v>
+        <v>8</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="65" ht="45">
@@ -2245,7 +2215,7 @@
         <v>3143379</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D65" s="2">
         <v>600</v>
@@ -2256,8 +2226,8 @@
       <c r="F65" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G65" s="2">
-        <v>0</v>
+      <c r="G65" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="66" ht="45">
@@ -2268,19 +2238,19 @@
         <v>3143380</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D66" s="2">
         <v>600</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G66" s="2">
-        <v>3.51</v>
+        <v>8</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="67" ht="45">
@@ -2291,7 +2261,7 @@
         <v>3143381</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D67" s="2">
         <v>3000</v>
@@ -2302,8 +2272,8 @@
       <c r="F67" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G67" s="2">
-        <v>0</v>
+      <c r="G67" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="68" ht="45">
@@ -2314,7 +2284,7 @@
         <v>3143382</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D68" s="2">
         <v>50</v>
@@ -2325,8 +2295,8 @@
       <c r="F68" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G68" s="2">
-        <v>0</v>
+      <c r="G68" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="69" ht="30">
@@ -2337,7 +2307,7 @@
         <v>3143383</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D69" s="2">
         <v>30</v>
@@ -2348,8 +2318,8 @@
       <c r="F69" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G69" s="2">
-        <v>0</v>
+      <c r="G69" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="70" ht="60">
@@ -2360,7 +2330,7 @@
         <v>3143384</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D70" s="2">
         <v>200</v>
@@ -2371,8 +2341,8 @@
       <c r="F70" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G70" s="2">
-        <v>0</v>
+      <c r="G70" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="71" ht="45">
@@ -2383,19 +2353,19 @@
         <v>3143385</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D71" s="2">
         <v>600</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G71" s="2">
-        <v>1.95</v>
+        <v>8</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="72" ht="30">
@@ -2406,7 +2376,7 @@
         <v>3143386</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D72" s="2">
         <v>3000</v>
@@ -2417,8 +2387,8 @@
       <c r="F72" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G72" s="2">
-        <v>0</v>
+      <c r="G72" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="73" ht="60">
@@ -2429,19 +2399,19 @@
         <v>3143387</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D73" s="2">
         <v>200</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G73" s="2">
-        <v>24.7</v>
+        <v>8</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="74" ht="45">
@@ -2452,7 +2422,7 @@
         <v>3143388</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D74" s="2">
         <v>200</v>
@@ -2463,8 +2433,8 @@
       <c r="F74" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G74" s="2">
-        <v>0</v>
+      <c r="G74" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="75" ht="45">
@@ -2475,19 +2445,19 @@
         <v>3143389</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D75" s="2">
         <v>400</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G75" s="2">
-        <v>2.08</v>
+        <v>8</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="76" ht="45">
@@ -2498,7 +2468,7 @@
         <v>3143390</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D76" s="2">
         <v>50</v>
@@ -2509,8 +2479,8 @@
       <c r="F76" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G76" s="2">
-        <v>0</v>
+      <c r="G76" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="77" ht="45">
@@ -2521,7 +2491,7 @@
         <v>3143391</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D77" s="2">
         <v>1000</v>
@@ -2532,8 +2502,8 @@
       <c r="F77" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G77" s="2">
-        <v>0</v>
+      <c r="G77" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="78" ht="45">
@@ -2544,7 +2514,7 @@
         <v>3143392</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D78" s="2">
         <v>200</v>
@@ -2555,8 +2525,8 @@
       <c r="F78" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G78" s="2">
-        <v>0</v>
+      <c r="G78" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="79" ht="45">
@@ -2567,7 +2537,7 @@
         <v>3143393</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D79" s="2">
         <v>100</v>
@@ -2578,8 +2548,8 @@
       <c r="F79" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G79" s="2">
-        <v>0</v>
+      <c r="G79" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="80" ht="45">
@@ -2590,7 +2560,7 @@
         <v>3143394</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D80" s="2">
         <v>200</v>
@@ -2601,8 +2571,8 @@
       <c r="F80" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G80" s="2">
-        <v>0</v>
+      <c r="G80" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="81" ht="45">
@@ -2613,19 +2583,19 @@
         <v>3143395</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D81" s="2">
         <v>800</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="G81" s="2">
-        <v>89.7</v>
+        <v>8</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="82" ht="45">
@@ -2636,19 +2606,19 @@
         <v>3143396</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D82" s="2">
         <v>15000</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="G82" s="2">
-        <v>29.9</v>
+        <v>8</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="83" ht="45">
@@ -2659,7 +2629,7 @@
         <v>3143397</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D83" s="2">
         <v>100</v>
@@ -2670,8 +2640,8 @@
       <c r="F83" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G83" s="2">
-        <v>0</v>
+      <c r="G83" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="84" ht="45">
@@ -2682,7 +2652,7 @@
         <v>3143398</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D84" s="2">
         <v>2000</v>
@@ -2693,8 +2663,8 @@
       <c r="F84" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G84" s="2">
-        <v>0</v>
+      <c r="G84" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="85" ht="45">
@@ -2705,7 +2675,7 @@
         <v>3143399</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D85" s="2">
         <v>200</v>
@@ -2716,8 +2686,8 @@
       <c r="F85" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G85" s="2">
-        <v>0</v>
+      <c r="G85" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="86" ht="45">
@@ -2728,7 +2698,7 @@
         <v>3143400</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D86" s="2">
         <v>200</v>
@@ -2739,8 +2709,8 @@
       <c r="F86" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G86" s="2">
-        <v>0</v>
+      <c r="G86" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="87" ht="45">
@@ -2751,7 +2721,7 @@
         <v>3143401</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D87" s="2">
         <v>600</v>
@@ -2762,8 +2732,8 @@
       <c r="F87" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G87" s="2">
-        <v>0</v>
+      <c r="G87" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="88" ht="45">
@@ -2774,7 +2744,7 @@
         <v>3143402</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D88" s="2">
         <v>400</v>
@@ -2785,8 +2755,8 @@
       <c r="F88" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G88" s="2">
-        <v>0</v>
+      <c r="G88" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="89" ht="45">
@@ -2797,7 +2767,7 @@
         <v>3143403</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D89" s="2">
         <v>100</v>
@@ -2808,8 +2778,8 @@
       <c r="F89" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G89" s="2">
-        <v>0</v>
+      <c r="G89" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="90" ht="45">
@@ -2820,7 +2790,7 @@
         <v>3143404</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D90" s="2">
         <v>1000</v>
@@ -2831,8 +2801,8 @@
       <c r="F90" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G90" s="2">
-        <v>0</v>
+      <c r="G90" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="91" ht="45">
@@ -2843,7 +2813,7 @@
         <v>3143405</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="D91" s="2">
         <v>20000</v>
@@ -2854,8 +2824,8 @@
       <c r="F91" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G91" s="2">
-        <v>0</v>
+      <c r="G91" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="92" ht="45">
@@ -2866,19 +2836,19 @@
         <v>3143406</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D92" s="2">
         <v>100</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G92" s="2">
-        <v>7.15</v>
+        <v>8</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="93" ht="45">
@@ -2889,7 +2859,7 @@
         <v>3143407</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D93" s="2">
         <v>100</v>
@@ -2900,8 +2870,8 @@
       <c r="F93" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G93" s="2">
-        <v>0</v>
+      <c r="G93" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="94" ht="45">
@@ -2912,19 +2882,19 @@
         <v>3143408</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D94" s="2">
         <v>1000</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F94" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G94" s="2">
-        <v>2.47</v>
+        <v>8</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="95" ht="45">
@@ -2935,7 +2905,7 @@
         <v>3143409</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="D95" s="2">
         <v>100</v>
@@ -2946,8 +2916,8 @@
       <c r="F95" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G95" s="2">
-        <v>0</v>
+      <c r="G95" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="96" ht="45">
@@ -2958,7 +2928,7 @@
         <v>3143410</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D96" s="2">
         <v>300</v>
@@ -2969,8 +2939,8 @@
       <c r="F96" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G96" s="2">
-        <v>0</v>
+      <c r="G96" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="97" ht="45">
@@ -2981,7 +2951,7 @@
         <v>3143411</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D97" s="2">
         <v>12000</v>
@@ -2992,8 +2962,8 @@
       <c r="F97" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G97" s="2">
-        <v>0</v>
+      <c r="G97" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="98" ht="45">
@@ -3004,7 +2974,7 @@
         <v>3143412</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D98" s="2">
         <v>6000</v>
@@ -3015,8 +2985,8 @@
       <c r="F98" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G98" s="2">
-        <v>0</v>
+      <c r="G98" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="99" ht="45">
@@ -3027,7 +2997,7 @@
         <v>3143413</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D99" s="2">
         <v>300</v>
@@ -3038,8 +3008,8 @@
       <c r="F99" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G99" s="2">
-        <v>0</v>
+      <c r="G99" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="100" ht="30">
@@ -3050,19 +3020,19 @@
         <v>3143414</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D100" s="2">
         <v>4000</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F100" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G100" s="2">
-        <v>1.24</v>
+        <v>8</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="101" ht="45">
@@ -3073,7 +3043,7 @@
         <v>3143415</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D101" s="2">
         <v>50</v>
@@ -3084,8 +3054,8 @@
       <c r="F101" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G101" s="2">
-        <v>0</v>
+      <c r="G101" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="102" ht="60">
@@ -3096,7 +3066,7 @@
         <v>3143416</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D102" s="2">
         <v>50</v>
@@ -3107,8 +3077,8 @@
       <c r="F102" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G102" s="2">
-        <v>0</v>
+      <c r="G102" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="103" ht="45">
@@ -3119,19 +3089,19 @@
         <v>3143417</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D103" s="2">
         <v>50</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="F103" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="G103" s="2">
-        <v>11.57</v>
+        <v>8</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="104" ht="45">
@@ -3142,7 +3112,7 @@
         <v>3143418</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D104" s="2">
         <v>200</v>
@@ -3153,8 +3123,8 @@
       <c r="F104" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G104" s="2">
-        <v>0</v>
+      <c r="G104" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="105" ht="45">
@@ -3165,7 +3135,7 @@
         <v>3143419</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D105" s="2">
         <v>300</v>
@@ -3176,8 +3146,8 @@
       <c r="F105" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G105" s="2">
-        <v>0</v>
+      <c r="G105" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="106" ht="45">
@@ -3188,7 +3158,7 @@
         <v>3143420</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D106" s="2">
         <v>1000</v>
@@ -3199,8 +3169,8 @@
       <c r="F106" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G106" s="2">
-        <v>0</v>
+      <c r="G106" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="107" ht="60">
@@ -3211,19 +3181,19 @@
         <v>3143421</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D107" s="2">
         <v>100</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F107" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G107" s="2">
-        <v>6.37</v>
+        <v>8</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="108" ht="45">
@@ -3234,19 +3204,19 @@
         <v>3143422</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D108" s="2">
         <v>4000</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F108" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G108" s="2">
-        <v>9.09</v>
+        <v>8</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="109" ht="45">
@@ -3257,7 +3227,7 @@
         <v>3143423</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D109" s="2">
         <v>2000</v>
@@ -3268,8 +3238,8 @@
       <c r="F109" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G109" s="2">
-        <v>0</v>
+      <c r="G109" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="110" ht="45">
@@ -3280,7 +3250,7 @@
         <v>3143424</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D110" s="2">
         <v>100</v>
@@ -3291,8 +3261,8 @@
       <c r="F110" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G110" s="2">
-        <v>0</v>
+      <c r="G110" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>